<commit_message>
CI: actualizar bases, hojas y reportes
</commit_message>
<xml_diff>
--- a/public_db/IMSA_DB.xlsx
+++ b/public_db/IMSA_DB.xlsx
@@ -15394,7 +15394,7 @@
         <xdr:cNvPr id="2" name="Picture 1" descr="logo.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15708,11 +15708,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J2659"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A2261" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2273" sqref="A2273"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A1850" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15.05"/>
@@ -15720,7 +15721,7 @@
     <col min="1" max="1" width="25.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.33203125" customWidth="1"/>
     <col min="3" max="3" width="31.5546875" customWidth="1"/>
-    <col min="4" max="4" width="45.5546875" customWidth="1"/>
+    <col min="4" max="4" width="68.109375" customWidth="1"/>
     <col min="5" max="5" width="17.6640625" style="9" customWidth="1"/>
     <col min="6" max="6" width="8.6640625" customWidth="1"/>
     <col min="7" max="7" width="17.6640625" style="9" customWidth="1"/>
@@ -15738,7 +15739,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="1"/>
       <c r="G1" s="10">
-        <v>45938</v>
+        <v>45939</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -15849,7 +15850,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" hidden="1">
       <c r="A8" t="s">
         <v>4485</v>
       </c>
@@ -16376,7 +16377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" hidden="1">
       <c r="A25" t="s">
         <v>519</v>
       </c>
@@ -16407,7 +16408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" hidden="1">
       <c r="A26" t="s">
         <v>879</v>
       </c>
@@ -16469,7 +16470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" hidden="1">
       <c r="A28" t="s">
         <v>1864</v>
       </c>
@@ -16500,7 +16501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" hidden="1">
       <c r="A29" t="s">
         <v>1962</v>
       </c>
@@ -16531,7 +16532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" hidden="1">
       <c r="A30" t="s">
         <v>743</v>
       </c>
@@ -16996,7 +16997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" hidden="1">
       <c r="A45" t="s">
         <v>2514</v>
       </c>
@@ -17058,7 +17059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" hidden="1">
       <c r="A47" t="s">
         <v>586</v>
       </c>
@@ -17182,7 +17183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" hidden="1">
       <c r="A51" t="s">
         <v>734</v>
       </c>
@@ -17213,7 +17214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" hidden="1">
       <c r="A52" t="s">
         <v>587</v>
       </c>
@@ -17275,7 +17276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" hidden="1">
       <c r="A54" t="s">
         <v>4889</v>
       </c>
@@ -17461,7 +17462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" hidden="1">
       <c r="A60" t="s">
         <v>4895</v>
       </c>
@@ -17802,7 +17803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" hidden="1">
       <c r="A71" t="s">
         <v>4217</v>
       </c>
@@ -18698,7 +18699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" hidden="1">
       <c r="A100" t="s">
         <v>4218</v>
       </c>
@@ -19408,7 +19409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" hidden="1">
       <c r="A123" t="s">
         <v>3794</v>
       </c>
@@ -19439,7 +19440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" hidden="1">
       <c r="A124" t="s">
         <v>3792</v>
       </c>
@@ -20493,7 +20494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" hidden="1">
       <c r="A158" t="s">
         <v>4203</v>
       </c>
@@ -20707,7 +20708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" hidden="1">
       <c r="A165" t="s">
         <v>4188</v>
       </c>
@@ -21200,7 +21201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" hidden="1">
       <c r="A181" t="s">
         <v>4416</v>
       </c>
@@ -21293,7 +21294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" hidden="1">
       <c r="A184" t="s">
         <v>1266</v>
       </c>
@@ -21324,7 +21325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" hidden="1">
       <c r="A185" t="s">
         <v>945</v>
       </c>
@@ -21355,7 +21356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" hidden="1">
       <c r="A186" t="s">
         <v>2957</v>
       </c>
@@ -21386,7 +21387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" hidden="1">
       <c r="A187" t="s">
         <v>2955</v>
       </c>
@@ -21417,7 +21418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" hidden="1">
       <c r="A188" t="s">
         <v>2953</v>
       </c>
@@ -21448,7 +21449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" hidden="1">
       <c r="A189" t="s">
         <v>692</v>
       </c>
@@ -21479,7 +21480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" hidden="1">
       <c r="A190" t="s">
         <v>4204</v>
       </c>
@@ -21507,7 +21508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" hidden="1">
       <c r="A191" t="s">
         <v>2413</v>
       </c>
@@ -21538,7 +21539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" hidden="1">
       <c r="A192" t="s">
         <v>4345</v>
       </c>
@@ -21597,7 +21598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" hidden="1">
       <c r="A194" t="s">
         <v>2567</v>
       </c>
@@ -21628,7 +21629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" hidden="1">
       <c r="A195" t="s">
         <v>4205</v>
       </c>
@@ -21873,7 +21874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" hidden="1">
       <c r="A203" t="s">
         <v>4189</v>
       </c>
@@ -22149,7 +22150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" hidden="1">
       <c r="A212" t="s">
         <v>2336</v>
       </c>
@@ -22738,7 +22739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" hidden="1">
       <c r="A231" t="s">
         <v>2054</v>
       </c>
@@ -24319,7 +24320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" hidden="1">
       <c r="A282" t="s">
         <v>3044</v>
       </c>
@@ -25373,7 +25374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:10">
+    <row r="316" spans="1:10" hidden="1">
       <c r="A316" t="s">
         <v>3767</v>
       </c>
@@ -25559,7 +25560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="322" spans="1:10">
+    <row r="322" spans="1:10" hidden="1">
       <c r="A322" t="s">
         <v>4963</v>
       </c>
@@ -27264,7 +27265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:10">
+    <row r="377" spans="1:10" hidden="1">
       <c r="A377" t="s">
         <v>4339</v>
       </c>
@@ -29744,7 +29745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="457" spans="1:10">
+    <row r="457" spans="1:10" hidden="1">
       <c r="A457" t="s">
         <v>4729</v>
       </c>
@@ -30798,7 +30799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="491" spans="1:10">
+    <row r="491" spans="1:10" hidden="1">
       <c r="A491" t="s">
         <v>627</v>
       </c>
@@ -31542,7 +31543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="515" spans="1:10">
+    <row r="515" spans="1:10" hidden="1">
       <c r="A515" t="s">
         <v>2872</v>
       </c>
@@ -31635,7 +31636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="518" spans="1:10">
+    <row r="518" spans="1:10" hidden="1">
       <c r="A518" t="s">
         <v>1924</v>
       </c>
@@ -31914,7 +31915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="527" spans="1:10">
+    <row r="527" spans="1:10" hidden="1">
       <c r="A527" t="s">
         <v>4340</v>
       </c>
@@ -32286,7 +32287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="539" spans="1:10">
+    <row r="539" spans="1:10" hidden="1">
       <c r="A539" t="s">
         <v>2913</v>
       </c>
@@ -32565,7 +32566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="548" spans="1:10">
+    <row r="548" spans="1:10" hidden="1">
       <c r="A548" t="s">
         <v>4489</v>
       </c>
@@ -35541,7 +35542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="644" spans="1:10">
+    <row r="644" spans="1:10" hidden="1">
       <c r="A644" t="s">
         <v>2760</v>
       </c>
@@ -35851,7 +35852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="654" spans="1:10">
+    <row r="654" spans="1:10" hidden="1">
       <c r="A654" t="s">
         <v>4341</v>
       </c>
@@ -36037,7 +36038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="660" spans="1:10">
+    <row r="660" spans="1:10" hidden="1">
       <c r="A660" t="s">
         <v>3944</v>
       </c>
@@ -37308,7 +37309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="701" spans="1:10">
+    <row r="701" spans="1:10" hidden="1">
       <c r="A701" t="s">
         <v>4119</v>
       </c>
@@ -40811,7 +40812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="814" spans="1:10">
+    <row r="814" spans="1:10" hidden="1">
       <c r="A814" t="s">
         <v>3763</v>
       </c>
@@ -41958,7 +41959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="851" spans="1:10">
+    <row r="851" spans="1:10" hidden="1">
       <c r="A851" t="s">
         <v>428</v>
       </c>
@@ -42175,7 +42176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="858" spans="1:10">
+    <row r="858" spans="1:10" hidden="1">
       <c r="A858" t="s">
         <v>744</v>
       </c>
@@ -42237,7 +42238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="860" spans="1:10">
+    <row r="860" spans="1:10" hidden="1">
       <c r="A860" t="s">
         <v>588</v>
       </c>
@@ -42392,7 +42393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="865" spans="1:10">
+    <row r="865" spans="1:10" hidden="1">
       <c r="A865" t="s">
         <v>18</v>
       </c>
@@ -43167,7 +43168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="890" spans="1:10">
+    <row r="890" spans="1:10" hidden="1">
       <c r="A890" t="s">
         <v>74</v>
       </c>
@@ -43198,7 +43199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="891" spans="1:10">
+    <row r="891" spans="1:10" hidden="1">
       <c r="A891" t="s">
         <v>227</v>
       </c>
@@ -43725,7 +43726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="908" spans="1:10">
+    <row r="908" spans="1:10" hidden="1">
       <c r="A908" t="s">
         <v>4350</v>
       </c>
@@ -45365,7 +45366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="961" spans="1:10">
+    <row r="961" spans="1:10" hidden="1">
       <c r="A961" t="s">
         <v>2883</v>
       </c>
@@ -45396,7 +45397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="962" spans="1:10">
+    <row r="962" spans="1:10" hidden="1">
       <c r="A962" t="s">
         <v>3529</v>
       </c>
@@ -45706,7 +45707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="972" spans="1:10">
+    <row r="972" spans="1:10" hidden="1">
       <c r="A972" t="s">
         <v>4195</v>
       </c>
@@ -46013,7 +46014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="982" spans="1:10">
+    <row r="982" spans="1:10" hidden="1">
       <c r="A982" t="s">
         <v>4199</v>
       </c>
@@ -46351,7 +46352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="993" spans="1:10">
+    <row r="993" spans="1:10" hidden="1">
       <c r="A993" t="s">
         <v>4351</v>
       </c>
@@ -46441,7 +46442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="996" spans="1:10">
+    <row r="996" spans="1:10" hidden="1">
       <c r="A996" t="s">
         <v>4200</v>
       </c>
@@ -48515,7 +48516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1063" spans="1:10">
+    <row r="1063" spans="1:10" hidden="1">
       <c r="A1063" t="s">
         <v>4201</v>
       </c>
@@ -48791,7 +48792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1072" spans="1:10">
+    <row r="1072" spans="1:10" hidden="1">
       <c r="A1072" t="s">
         <v>2885</v>
       </c>
@@ -49070,7 +49071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1081" spans="1:10">
+    <row r="1081" spans="1:10" hidden="1">
       <c r="A1081" t="s">
         <v>2887</v>
       </c>
@@ -50093,7 +50094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1114" spans="1:10">
+    <row r="1114" spans="1:10" hidden="1">
       <c r="A1114" t="s">
         <v>2361</v>
       </c>
@@ -50124,7 +50125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1115" spans="1:10">
+    <row r="1115" spans="1:10" hidden="1">
       <c r="A1115" t="s">
         <v>2338</v>
       </c>
@@ -50279,7 +50280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1120" spans="1:10">
+    <row r="1120" spans="1:10" hidden="1">
       <c r="A1120" t="s">
         <v>4202</v>
       </c>
@@ -50493,7 +50494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1127" spans="1:10">
+    <row r="1127" spans="1:10" hidden="1">
       <c r="A1127" t="s">
         <v>4352</v>
       </c>
@@ -50617,7 +50618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1131" spans="1:10">
+    <row r="1131" spans="1:10" hidden="1">
       <c r="A1131" t="s">
         <v>1720</v>
       </c>
@@ -52756,7 +52757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1200" spans="1:10">
+    <row r="1200" spans="1:10" hidden="1">
       <c r="A1200" t="s">
         <v>4354</v>
       </c>
@@ -53497,7 +53498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1224" spans="1:10">
+    <row r="1224" spans="1:10" hidden="1">
       <c r="A1224" t="s">
         <v>2723</v>
       </c>
@@ -54334,7 +54335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1251" spans="1:10">
+    <row r="1251" spans="1:10" hidden="1">
       <c r="A1251" t="s">
         <v>4355</v>
       </c>
@@ -55605,7 +55606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1292" spans="1:10">
+    <row r="1292" spans="1:10" hidden="1">
       <c r="A1292" t="s">
         <v>1388</v>
       </c>
@@ -55853,7 +55854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1300" spans="1:10">
+    <row r="1300" spans="1:10" hidden="1">
       <c r="A1300" t="s">
         <v>2959</v>
       </c>
@@ -55912,7 +55913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1302" spans="1:10">
+    <row r="1302" spans="1:10" hidden="1">
       <c r="A1302" t="s">
         <v>4206</v>
       </c>
@@ -55940,7 +55941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1303" spans="1:10">
+    <row r="1303" spans="1:10" hidden="1">
       <c r="A1303" t="s">
         <v>2278</v>
       </c>
@@ -55971,7 +55972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1304" spans="1:10">
+    <row r="1304" spans="1:10" hidden="1">
       <c r="A1304" t="s">
         <v>2915</v>
       </c>
@@ -56002,7 +56003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1305" spans="1:10">
+    <row r="1305" spans="1:10" hidden="1">
       <c r="A1305" t="s">
         <v>2951</v>
       </c>
@@ -56033,7 +56034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1306" spans="1:10">
+    <row r="1306" spans="1:10" hidden="1">
       <c r="A1306" t="s">
         <v>2949</v>
       </c>
@@ -56467,7 +56468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1320" spans="1:10">
+    <row r="1320" spans="1:10" hidden="1">
       <c r="A1320" t="s">
         <v>1068</v>
       </c>
@@ -56529,7 +56530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1322" spans="1:10">
+    <row r="1322" spans="1:10" hidden="1">
       <c r="A1322" t="s">
         <v>3445</v>
       </c>
@@ -56560,7 +56561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1323" spans="1:10">
+    <row r="1323" spans="1:10" hidden="1">
       <c r="A1323" t="s">
         <v>2005</v>
       </c>
@@ -56715,7 +56716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1328" spans="1:10">
+    <row r="1328" spans="1:10" hidden="1">
       <c r="A1328" t="s">
         <v>4346</v>
       </c>
@@ -56743,7 +56744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1329" spans="1:10">
+    <row r="1329" spans="1:10" hidden="1">
       <c r="A1329" t="s">
         <v>469</v>
       </c>
@@ -56774,7 +56775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1330" spans="1:10">
+    <row r="1330" spans="1:10" hidden="1">
       <c r="A1330" t="s">
         <v>403</v>
       </c>
@@ -56805,7 +56806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1331" spans="1:10">
+    <row r="1331" spans="1:10" hidden="1">
       <c r="A1331" t="s">
         <v>4207</v>
       </c>
@@ -56864,7 +56865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1333" spans="1:10">
+    <row r="1333" spans="1:10" hidden="1">
       <c r="A1333" t="s">
         <v>4209</v>
       </c>
@@ -56895,7 +56896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1334" spans="1:10">
+    <row r="1334" spans="1:10" hidden="1">
       <c r="A1334" t="s">
         <v>4186</v>
       </c>
@@ -57143,7 +57144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1342" spans="1:10">
+    <row r="1342" spans="1:10" hidden="1">
       <c r="A1342" t="s">
         <v>4196</v>
       </c>
@@ -59775,7 +59776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1427" spans="1:10">
+    <row r="1427" spans="1:10" hidden="1">
       <c r="A1427" t="s">
         <v>4434</v>
       </c>
@@ -59837,7 +59838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1429" spans="1:10">
+    <row r="1429" spans="1:10" hidden="1">
       <c r="A1429" t="s">
         <v>4432</v>
       </c>
@@ -60984,7 +60985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1466" spans="1:10">
+    <row r="1466" spans="1:10" hidden="1">
       <c r="A1466" t="s">
         <v>618</v>
       </c>
@@ -61077,7 +61078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1469" spans="1:10">
+    <row r="1469" spans="1:10" hidden="1">
       <c r="A1469" t="s">
         <v>681</v>
       </c>
@@ -61139,7 +61140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1471" spans="1:10">
+    <row r="1471" spans="1:10" hidden="1">
       <c r="A1471" t="s">
         <v>1478</v>
       </c>
@@ -61201,7 +61202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1473" spans="1:10">
+    <row r="1473" spans="1:10" hidden="1">
       <c r="A1473" t="s">
         <v>1492</v>
       </c>
@@ -61232,7 +61233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1474" spans="1:10">
+    <row r="1474" spans="1:10" hidden="1">
       <c r="A1474" t="s">
         <v>541</v>
       </c>
@@ -61263,7 +61264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1475" spans="1:10">
+    <row r="1475" spans="1:10" hidden="1">
       <c r="A1475" t="s">
         <v>3809</v>
       </c>
@@ -61418,7 +61419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1480" spans="1:10">
+    <row r="1480" spans="1:10" hidden="1">
       <c r="A1480" t="s">
         <v>2909</v>
       </c>
@@ -61449,7 +61450,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1481" spans="1:10">
+    <row r="1481" spans="1:10" hidden="1">
       <c r="A1481" t="s">
         <v>2911</v>
       </c>
@@ -61542,7 +61543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1484" spans="1:10">
+    <row r="1484" spans="1:10" hidden="1">
       <c r="A1484" t="s">
         <v>3075</v>
       </c>
@@ -61573,7 +61574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1485" spans="1:10">
+    <row r="1485" spans="1:10" hidden="1">
       <c r="A1485" t="s">
         <v>3082</v>
       </c>
@@ -61604,7 +61605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1486" spans="1:10">
+    <row r="1486" spans="1:10" hidden="1">
       <c r="A1486" t="s">
         <v>3079</v>
       </c>
@@ -61635,7 +61636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1487" spans="1:10">
+    <row r="1487" spans="1:10" hidden="1">
       <c r="A1487" t="s">
         <v>3314</v>
       </c>
@@ -61666,7 +61667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1488" spans="1:10">
+    <row r="1488" spans="1:10" hidden="1">
       <c r="A1488" t="s">
         <v>4406</v>
       </c>
@@ -61697,7 +61698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1489" spans="1:10">
+    <row r="1489" spans="1:10" hidden="1">
       <c r="A1489" t="s">
         <v>4408</v>
       </c>
@@ -61728,7 +61729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1490" spans="1:10">
+    <row r="1490" spans="1:10" hidden="1">
       <c r="A1490" t="s">
         <v>3086</v>
       </c>
@@ -61759,7 +61760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1491" spans="1:10">
+    <row r="1491" spans="1:10" hidden="1">
       <c r="A1491" t="s">
         <v>3090</v>
       </c>
@@ -61790,7 +61791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1492" spans="1:10">
+    <row r="1492" spans="1:10" hidden="1">
       <c r="A1492" t="s">
         <v>498</v>
       </c>
@@ -61821,7 +61822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1493" spans="1:10">
+    <row r="1493" spans="1:10" hidden="1">
       <c r="A1493" t="s">
         <v>1424</v>
       </c>
@@ -62348,7 +62349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1510" spans="1:10">
+    <row r="1510" spans="1:10" hidden="1">
       <c r="A1510" t="s">
         <v>763</v>
       </c>
@@ -62441,7 +62442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1513" spans="1:10">
+    <row r="1513" spans="1:10" hidden="1">
       <c r="A1513" t="s">
         <v>2417</v>
       </c>
@@ -62472,7 +62473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1514" spans="1:10">
+    <row r="1514" spans="1:10" hidden="1">
       <c r="A1514" t="s">
         <v>346</v>
       </c>
@@ -63123,7 +63124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1535" spans="1:10">
+    <row r="1535" spans="1:10" hidden="1">
       <c r="A1535" t="s">
         <v>3762</v>
       </c>
@@ -63154,7 +63155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1536" spans="1:10">
+    <row r="1536" spans="1:10" hidden="1">
       <c r="A1536" t="s">
         <v>3813</v>
       </c>
@@ -63185,7 +63186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1537" spans="1:10">
+    <row r="1537" spans="1:10" hidden="1">
       <c r="A1537" t="s">
         <v>3760</v>
       </c>
@@ -63216,7 +63217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1538" spans="1:10">
+    <row r="1538" spans="1:10" hidden="1">
       <c r="A1538" t="s">
         <v>3814</v>
       </c>
@@ -63402,7 +63403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1544" spans="1:10">
+    <row r="1544" spans="1:10" hidden="1">
       <c r="A1544" t="s">
         <v>4483</v>
       </c>
@@ -63433,7 +63434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1545" spans="1:10">
+    <row r="1545" spans="1:10" hidden="1">
       <c r="A1545" t="s">
         <v>3179</v>
       </c>
@@ -63464,7 +63465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1546" spans="1:10">
+    <row r="1546" spans="1:10" hidden="1">
       <c r="A1546" t="s">
         <v>3754</v>
       </c>
@@ -63495,7 +63496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1547" spans="1:10">
+    <row r="1547" spans="1:10" hidden="1">
       <c r="A1547" t="s">
         <v>3756</v>
       </c>
@@ -63526,7 +63527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1548" spans="1:10">
+    <row r="1548" spans="1:10" hidden="1">
       <c r="A1548" t="s">
         <v>3758</v>
       </c>
@@ -63712,7 +63713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1554" spans="1:10">
+    <row r="1554" spans="1:10" hidden="1">
       <c r="A1554" t="s">
         <v>2960</v>
       </c>
@@ -63743,7 +63744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1555" spans="1:10">
+    <row r="1555" spans="1:10" hidden="1">
       <c r="A1555" t="s">
         <v>3071</v>
       </c>
@@ -63774,7 +63775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1556" spans="1:10">
+    <row r="1556" spans="1:10" hidden="1">
       <c r="A1556" t="s">
         <v>3440</v>
       </c>
@@ -63805,7 +63806,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1557" spans="1:10">
+    <row r="1557" spans="1:10" hidden="1">
       <c r="A1557" t="s">
         <v>1860</v>
       </c>
@@ -63836,7 +63837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1558" spans="1:10">
+    <row r="1558" spans="1:10" hidden="1">
       <c r="A1558" t="s">
         <v>955</v>
       </c>
@@ -63867,7 +63868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1559" spans="1:10">
+    <row r="1559" spans="1:10" hidden="1">
       <c r="A1559" t="s">
         <v>1556</v>
       </c>
@@ -63898,7 +63899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1560" spans="1:10">
+    <row r="1560" spans="1:10" hidden="1">
       <c r="A1560" t="s">
         <v>2683</v>
       </c>
@@ -63929,7 +63930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1561" spans="1:10">
+    <row r="1561" spans="1:10" hidden="1">
       <c r="A1561" t="s">
         <v>791</v>
       </c>
@@ -63960,7 +63961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1562" spans="1:10">
+    <row r="1562" spans="1:10" hidden="1">
       <c r="A1562" t="s">
         <v>2118</v>
       </c>
@@ -63991,7 +63992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1563" spans="1:10">
+    <row r="1563" spans="1:10" hidden="1">
       <c r="A1563" t="s">
         <v>1558</v>
       </c>
@@ -64022,7 +64023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1564" spans="1:10">
+    <row r="1564" spans="1:10" hidden="1">
       <c r="A1564" t="s">
         <v>2907</v>
       </c>
@@ -64053,7 +64054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1565" spans="1:10">
+    <row r="1565" spans="1:10" hidden="1">
       <c r="A1565" t="s">
         <v>2705</v>
       </c>
@@ -64084,7 +64085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1566" spans="1:10">
+    <row r="1566" spans="1:10" hidden="1">
       <c r="A1566" t="s">
         <v>4481</v>
       </c>
@@ -64115,7 +64116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1567" spans="1:10">
+    <row r="1567" spans="1:10" hidden="1">
       <c r="A1567" t="s">
         <v>509</v>
       </c>
@@ -64580,7 +64581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1582" spans="1:10">
+    <row r="1582" spans="1:10" hidden="1">
       <c r="A1582" t="s">
         <v>1711</v>
       </c>
@@ -65076,7 +65077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1598" spans="1:10">
+    <row r="1598" spans="1:10" hidden="1">
       <c r="A1598" t="s">
         <v>1707</v>
       </c>
@@ -65479,7 +65480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1611" spans="1:10">
+    <row r="1611" spans="1:10" hidden="1">
       <c r="A1611" t="s">
         <v>3946</v>
       </c>
@@ -65758,7 +65759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1620" spans="1:10">
+    <row r="1620" spans="1:10" hidden="1">
       <c r="A1620" t="s">
         <v>1323</v>
       </c>
@@ -65882,7 +65883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1624" spans="1:10">
+    <row r="1624" spans="1:10" hidden="1">
       <c r="A1624" t="s">
         <v>698</v>
       </c>
@@ -66006,7 +66007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1628" spans="1:10">
+    <row r="1628" spans="1:10" hidden="1">
       <c r="A1628" t="s">
         <v>1709</v>
       </c>
@@ -66471,7 +66472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1643" spans="1:10">
+    <row r="1643" spans="1:10" hidden="1">
       <c r="A1643" t="s">
         <v>1422</v>
       </c>
@@ -69850,7 +69851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1752" spans="1:10">
+    <row r="1752" spans="1:10" hidden="1">
       <c r="A1752" t="s">
         <v>1098</v>
       </c>
@@ -70346,7 +70347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1768" spans="1:10">
+    <row r="1768" spans="1:10" hidden="1">
       <c r="A1768" t="s">
         <v>3043</v>
       </c>
@@ -70377,7 +70378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1769" spans="1:10">
+    <row r="1769" spans="1:10" hidden="1">
       <c r="A1769" t="s">
         <v>1442</v>
       </c>
@@ -70563,7 +70564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1775" spans="1:10">
+    <row r="1775" spans="1:10" hidden="1">
       <c r="A1775" t="s">
         <v>1791</v>
       </c>
@@ -70749,7 +70750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1781" spans="1:10">
+    <row r="1781" spans="1:10" hidden="1">
       <c r="A1781" t="s">
         <v>4216</v>
       </c>
@@ -70811,7 +70812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1783" spans="1:10">
+    <row r="1783" spans="1:10" hidden="1">
       <c r="A1783" t="s">
         <v>3645</v>
       </c>
@@ -70873,7 +70874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1785" spans="1:10">
+    <row r="1785" spans="1:10" hidden="1">
       <c r="A1785" t="s">
         <v>4440</v>
       </c>
@@ -70997,7 +70998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1789" spans="1:10">
+    <row r="1789" spans="1:10" hidden="1">
       <c r="A1789" t="s">
         <v>504</v>
       </c>
@@ -71028,7 +71029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1790" spans="1:10">
+    <row r="1790" spans="1:10" hidden="1">
       <c r="A1790" t="s">
         <v>952</v>
       </c>
@@ -71245,7 +71246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1797" spans="1:10">
+    <row r="1797" spans="1:10" hidden="1">
       <c r="A1797" t="s">
         <v>2086</v>
       </c>
@@ -71555,7 +71556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1807" spans="1:10">
+    <row r="1807" spans="1:10" hidden="1">
       <c r="A1807" t="s">
         <v>1096</v>
       </c>
@@ -71586,7 +71587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1808" spans="1:10">
+    <row r="1808" spans="1:10" hidden="1">
       <c r="A1808" t="s">
         <v>2947</v>
       </c>
@@ -72733,7 +72734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1845" spans="1:10">
+    <row r="1845" spans="1:10" hidden="1">
       <c r="A1845" t="s">
         <v>614</v>
       </c>
@@ -73159,8 +73160,8 @@
       <c r="G1858" s="9">
         <v>1610000</v>
       </c>
-      <c r="H1858" s="5" t="s">
-        <v>5080</v>
+      <c r="H1858" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="J1858" s="9">
         <f t="shared" si="59"/>
@@ -74097,7 +74098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1889" spans="1:10">
+    <row r="1889" spans="1:10" hidden="1">
       <c r="A1889" t="s">
         <v>4444</v>
       </c>
@@ -74714,7 +74715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1909" spans="1:10">
+    <row r="1909" spans="1:10" hidden="1">
       <c r="A1909" t="s">
         <v>2177</v>
       </c>
@@ -74838,7 +74839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1913" spans="1:10">
+    <row r="1913" spans="1:10" hidden="1">
       <c r="A1913" t="s">
         <v>1100</v>
       </c>
@@ -75334,7 +75335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1929" spans="1:10">
+    <row r="1929" spans="1:10" hidden="1">
       <c r="A1929" t="s">
         <v>2213</v>
       </c>
@@ -75365,7 +75366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1930" spans="1:10">
+    <row r="1930" spans="1:10" hidden="1">
       <c r="A1930" t="s">
         <v>854</v>
       </c>
@@ -75396,7 +75397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1931" spans="1:10">
+    <row r="1931" spans="1:10" hidden="1">
       <c r="A1931" t="s">
         <v>1854</v>
       </c>
@@ -75427,7 +75428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1932" spans="1:10">
+    <row r="1932" spans="1:10" hidden="1">
       <c r="A1932" t="s">
         <v>1476</v>
       </c>
@@ -75458,7 +75459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1933" spans="1:10">
+    <row r="1933" spans="1:10" hidden="1">
       <c r="A1933" t="s">
         <v>1852</v>
       </c>
@@ -75706,7 +75707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1941" spans="1:10">
+    <row r="1941" spans="1:10" hidden="1">
       <c r="A1941" t="s">
         <v>1960</v>
       </c>
@@ -75799,7 +75800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1944" spans="1:10">
+    <row r="1944" spans="1:10" hidden="1">
       <c r="A1944" t="s">
         <v>885</v>
       </c>
@@ -75954,7 +75955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1949" spans="1:10">
+    <row r="1949" spans="1:10" hidden="1">
       <c r="A1949" t="s">
         <v>903</v>
       </c>
@@ -75985,7 +75986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1950" spans="1:10">
+    <row r="1950" spans="1:10" hidden="1">
       <c r="A1950" t="s">
         <v>845</v>
       </c>
@@ -76047,7 +76048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1952" spans="1:10">
+    <row r="1952" spans="1:10" hidden="1">
       <c r="A1952" t="s">
         <v>866</v>
       </c>
@@ -76078,7 +76079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1953" spans="1:10">
+    <row r="1953" spans="1:10" hidden="1">
       <c r="A1953" t="s">
         <v>1497</v>
       </c>
@@ -76202,7 +76203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1957" spans="1:10">
+    <row r="1957" spans="1:10" hidden="1">
       <c r="A1957" t="s">
         <v>2106</v>
       </c>
@@ -76233,7 +76234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1958" spans="1:10">
+    <row r="1958" spans="1:10" hidden="1">
       <c r="A1958" t="s">
         <v>878</v>
       </c>
@@ -76698,7 +76699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1973" spans="1:10">
+    <row r="1973" spans="1:10" hidden="1">
       <c r="A1973" t="s">
         <v>898</v>
       </c>
@@ -76822,7 +76823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1977" spans="1:10">
+    <row r="1977" spans="1:10" hidden="1">
       <c r="A1977" t="s">
         <v>1790</v>
       </c>
@@ -77039,7 +77040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1984" spans="1:10">
+    <row r="1984" spans="1:10" hidden="1">
       <c r="A1984" t="s">
         <v>4344</v>
       </c>
@@ -77129,7 +77130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1987" spans="1:10">
+    <row r="1987" spans="1:10" hidden="1">
       <c r="A1987" t="s">
         <v>1499</v>
       </c>
@@ -77160,7 +77161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1988" spans="1:10">
+    <row r="1988" spans="1:10" hidden="1">
       <c r="A1988" t="s">
         <v>864</v>
       </c>
@@ -77191,7 +77192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1989" spans="1:10">
+    <row r="1989" spans="1:10" hidden="1">
       <c r="A1989" t="s">
         <v>1494</v>
       </c>
@@ -77222,7 +77223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1990" spans="1:10">
+    <row r="1990" spans="1:10" hidden="1">
       <c r="A1990" t="s">
         <v>2419</v>
       </c>
@@ -77253,7 +77254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1991" spans="1:10">
+    <row r="1991" spans="1:10" hidden="1">
       <c r="A1991" t="s">
         <v>883</v>
       </c>
@@ -77284,7 +77285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1992" spans="1:10">
+    <row r="1992" spans="1:10" hidden="1">
       <c r="A1992" t="s">
         <v>881</v>
       </c>
@@ -77346,7 +77347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1994" spans="1:10">
+    <row r="1994" spans="1:10" hidden="1">
       <c r="A1994" t="s">
         <v>862</v>
       </c>
@@ -77687,7 +77688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2005" spans="1:10">
+    <row r="2005" spans="1:10" hidden="1">
       <c r="A2005" t="s">
         <v>2144</v>
       </c>
@@ -77749,7 +77750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2007" spans="1:10">
+    <row r="2007" spans="1:10" hidden="1">
       <c r="A2007" t="s">
         <v>860</v>
       </c>
@@ -77780,7 +77781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2008" spans="1:10">
+    <row r="2008" spans="1:10" hidden="1">
       <c r="A2008" t="s">
         <v>887</v>
       </c>
@@ -77935,7 +77936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2013" spans="1:10">
+    <row r="2013" spans="1:10" hidden="1">
       <c r="A2013" t="s">
         <v>856</v>
       </c>
@@ -78059,7 +78060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2017" spans="1:10">
+    <row r="2017" spans="1:10" hidden="1">
       <c r="A2017" t="s">
         <v>629</v>
       </c>
@@ -78152,7 +78153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2020" spans="1:10">
+    <row r="2020" spans="1:10" hidden="1">
       <c r="A2020" t="s">
         <v>622</v>
       </c>
@@ -78369,7 +78370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2027" spans="1:10">
+    <row r="2027" spans="1:10" hidden="1">
       <c r="A2027" t="s">
         <v>1866</v>
       </c>
@@ -78772,7 +78773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2040" spans="1:10">
+    <row r="2040" spans="1:10" hidden="1">
       <c r="A2040" t="s">
         <v>759</v>
       </c>
@@ -78803,7 +78804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2041" spans="1:10">
+    <row r="2041" spans="1:10" hidden="1">
       <c r="A2041" t="s">
         <v>1443</v>
       </c>
@@ -79237,7 +79238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2055" spans="1:10">
+    <row r="2055" spans="1:10" hidden="1">
       <c r="A2055" t="s">
         <v>1884</v>
       </c>
@@ -79330,7 +79331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2058" spans="1:10">
+    <row r="2058" spans="1:10" hidden="1">
       <c r="A2058" t="s">
         <v>590</v>
       </c>
@@ -79361,7 +79362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2059" spans="1:10">
+    <row r="2059" spans="1:10" hidden="1">
       <c r="A2059" t="s">
         <v>1920</v>
       </c>
@@ -79454,7 +79455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2062" spans="1:10">
+    <row r="2062" spans="1:10" hidden="1">
       <c r="A2062" t="s">
         <v>1922</v>
       </c>
@@ -80012,7 +80013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2080" spans="1:10">
+    <row r="2080" spans="1:10" hidden="1">
       <c r="A2080" t="s">
         <v>3442</v>
       </c>
@@ -80136,7 +80137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2084" spans="1:10">
+    <row r="2084" spans="1:10" hidden="1">
       <c r="A2084" t="s">
         <v>2062</v>
       </c>
@@ -80167,7 +80168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2085" spans="1:10">
+    <row r="2085" spans="1:10" hidden="1">
       <c r="A2085" t="s">
         <v>2108</v>
       </c>
@@ -80229,7 +80230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2087" spans="1:10">
+    <row r="2087" spans="1:10" hidden="1">
       <c r="A2087" t="s">
         <v>4197</v>
       </c>
@@ -80973,7 +80974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2111" spans="1:10">
+    <row r="2111" spans="1:10" hidden="1">
       <c r="A2111" t="s">
         <v>1500</v>
       </c>
@@ -81190,7 +81191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2118" spans="1:10">
+    <row r="2118" spans="1:10" hidden="1">
       <c r="A2118" t="s">
         <v>953</v>
       </c>
@@ -81531,7 +81532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2129" spans="1:10">
+    <row r="2129" spans="1:10" hidden="1">
       <c r="A2129" t="s">
         <v>838</v>
       </c>
@@ -81593,7 +81594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2131" spans="1:10">
+    <row r="2131" spans="1:10" hidden="1">
       <c r="A2131" t="s">
         <v>972</v>
       </c>
@@ -81624,7 +81625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2132" spans="1:10">
+    <row r="2132" spans="1:10" hidden="1">
       <c r="A2132" t="s">
         <v>970</v>
       </c>
@@ -82027,7 +82028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2145" spans="1:10">
+    <row r="2145" spans="1:10" hidden="1">
       <c r="A2145" t="s">
         <v>4334</v>
       </c>
@@ -84011,7 +84012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2209" spans="1:10">
+    <row r="2209" spans="1:10" hidden="1">
       <c r="A2209" t="s">
         <v>1354</v>
       </c>
@@ -84073,7 +84074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2211" spans="1:10">
+    <row r="2211" spans="1:10" hidden="1">
       <c r="A2211" t="s">
         <v>3931</v>
       </c>
@@ -84507,7 +84508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2225" spans="1:10">
+    <row r="2225" spans="1:10" hidden="1">
       <c r="A2225" t="s">
         <v>4507</v>
       </c>
@@ -85561,7 +85562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2259" spans="1:10">
+    <row r="2259" spans="1:10" hidden="1">
       <c r="A2259" t="s">
         <v>4445</v>
       </c>
@@ -85592,7 +85593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2260" spans="1:10">
+    <row r="2260" spans="1:10" hidden="1">
       <c r="A2260" t="s">
         <v>4190</v>
       </c>
@@ -87387,7 +87388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2318" spans="1:10">
+    <row r="2318" spans="1:10" hidden="1">
       <c r="A2318" t="s">
         <v>4233</v>
       </c>
@@ -88035,7 +88036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2339" spans="1:10">
+    <row r="2339" spans="1:10" hidden="1">
       <c r="A2339" t="s">
         <v>4347</v>
       </c>
@@ -88497,7 +88498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2354" spans="1:10">
+    <row r="2354" spans="1:10" hidden="1">
       <c r="A2354" t="s">
         <v>4525</v>
       </c>
@@ -88559,7 +88560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2356" spans="1:10">
+    <row r="2356" spans="1:10" hidden="1">
       <c r="A2356" t="s">
         <v>1420</v>
       </c>
@@ -88621,7 +88622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2358" spans="1:10">
+    <row r="2358" spans="1:10" hidden="1">
       <c r="A2358" t="s">
         <v>4527</v>
       </c>
@@ -88900,7 +88901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2367" spans="1:10">
+    <row r="2367" spans="1:10" hidden="1">
       <c r="A2367" t="s">
         <v>4531</v>
       </c>
@@ -89303,7 +89304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2380" spans="1:10">
+    <row r="2380" spans="1:10" hidden="1">
       <c r="A2380" t="s">
         <v>4348</v>
       </c>
@@ -89331,7 +89332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2381" spans="1:10">
+    <row r="2381" spans="1:10" hidden="1">
       <c r="A2381" t="s">
         <v>2931</v>
       </c>
@@ -89641,7 +89642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2391" spans="1:10">
+    <row r="2391" spans="1:10" hidden="1">
       <c r="A2391" t="s">
         <v>2363</v>
       </c>
@@ -89672,7 +89673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2392" spans="1:10">
+    <row r="2392" spans="1:10" hidden="1">
       <c r="A2392" t="s">
         <v>2365</v>
       </c>
@@ -89703,7 +89704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2393" spans="1:10">
+    <row r="2393" spans="1:10" hidden="1">
       <c r="A2393" t="s">
         <v>4117</v>
       </c>
@@ -89734,7 +89735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2394" spans="1:10">
+    <row r="2394" spans="1:10" hidden="1">
       <c r="A2394" t="s">
         <v>2367</v>
       </c>
@@ -89796,7 +89797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2396" spans="1:10">
+    <row r="2396" spans="1:10" hidden="1">
       <c r="A2396" t="s">
         <v>2375</v>
       </c>
@@ -89827,7 +89828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2397" spans="1:10">
+    <row r="2397" spans="1:10" hidden="1">
       <c r="A2397" t="s">
         <v>4090</v>
       </c>
@@ -89858,7 +89859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2398" spans="1:10">
+    <row r="2398" spans="1:10" hidden="1">
       <c r="A2398" t="s">
         <v>4092</v>
       </c>
@@ -89889,7 +89890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2399" spans="1:10">
+    <row r="2399" spans="1:10" hidden="1">
       <c r="A2399" t="s">
         <v>2377</v>
       </c>
@@ -89920,7 +89921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2400" spans="1:10">
+    <row r="2400" spans="1:10" hidden="1">
       <c r="A2400" t="s">
         <v>4094</v>
       </c>
@@ -89951,7 +89952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2401" spans="1:10">
+    <row r="2401" spans="1:10" hidden="1">
       <c r="A2401" t="s">
         <v>4096</v>
       </c>
@@ -89982,7 +89983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2402" spans="1:10">
+    <row r="2402" spans="1:10" hidden="1">
       <c r="A2402" t="s">
         <v>2379</v>
       </c>
@@ -90013,7 +90014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2403" spans="1:10">
+    <row r="2403" spans="1:10" hidden="1">
       <c r="A2403" t="s">
         <v>4098</v>
       </c>
@@ -90075,7 +90076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2405" spans="1:10">
+    <row r="2405" spans="1:10" hidden="1">
       <c r="A2405" t="s">
         <v>2373</v>
       </c>
@@ -90106,7 +90107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2406" spans="1:10">
+    <row r="2406" spans="1:10" hidden="1">
       <c r="A2406" t="s">
         <v>4070</v>
       </c>
@@ -90137,7 +90138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2407" spans="1:10">
+    <row r="2407" spans="1:10" hidden="1">
       <c r="A2407" t="s">
         <v>3366</v>
       </c>
@@ -90168,7 +90169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2408" spans="1:10">
+    <row r="2408" spans="1:10" hidden="1">
       <c r="A2408" t="s">
         <v>4100</v>
       </c>
@@ -90199,7 +90200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2409" spans="1:10">
+    <row r="2409" spans="1:10" hidden="1">
       <c r="A2409" t="s">
         <v>2387</v>
       </c>
@@ -90230,7 +90231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2410" spans="1:10">
+    <row r="2410" spans="1:10" hidden="1">
       <c r="A2410" t="s">
         <v>3360</v>
       </c>
@@ -90261,7 +90262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2411" spans="1:10">
+    <row r="2411" spans="1:10" hidden="1">
       <c r="A2411" t="s">
         <v>4104</v>
       </c>
@@ -90292,7 +90293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2412" spans="1:10">
+    <row r="2412" spans="1:10" hidden="1">
       <c r="A2412" t="s">
         <v>2385</v>
       </c>
@@ -90323,7 +90324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2413" spans="1:10">
+    <row r="2413" spans="1:10" hidden="1">
       <c r="A2413" t="s">
         <v>4107</v>
       </c>
@@ -90354,7 +90355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2414" spans="1:10">
+    <row r="2414" spans="1:10" hidden="1">
       <c r="A2414" t="s">
         <v>4106</v>
       </c>
@@ -90385,7 +90386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2415" spans="1:10">
+    <row r="2415" spans="1:10" hidden="1">
       <c r="A2415" t="s">
         <v>4109</v>
       </c>
@@ -90416,7 +90417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2416" spans="1:10">
+    <row r="2416" spans="1:10" hidden="1">
       <c r="A2416" t="s">
         <v>2383</v>
       </c>
@@ -90447,7 +90448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2417" spans="1:10">
+    <row r="2417" spans="1:10" hidden="1">
       <c r="A2417" t="s">
         <v>4111</v>
       </c>
@@ -90478,7 +90479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2418" spans="1:10">
+    <row r="2418" spans="1:10" hidden="1">
       <c r="A2418" t="s">
         <v>4113</v>
       </c>
@@ -90509,7 +90510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2419" spans="1:10">
+    <row r="2419" spans="1:10" hidden="1">
       <c r="A2419" t="s">
         <v>2381</v>
       </c>
@@ -90664,7 +90665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2424" spans="1:10">
+    <row r="2424" spans="1:10" hidden="1">
       <c r="A2424" t="s">
         <v>4585</v>
       </c>
@@ -90943,7 +90944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2433" spans="1:10">
+    <row r="2433" spans="1:10" hidden="1">
       <c r="A2433" t="s">
         <v>3672</v>
       </c>
@@ -90974,7 +90975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2434" spans="1:10">
+    <row r="2434" spans="1:10" hidden="1">
       <c r="A2434" t="s">
         <v>4559</v>
       </c>
@@ -91191,7 +91192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2441" spans="1:10">
+    <row r="2441" spans="1:10" hidden="1">
       <c r="A2441" t="s">
         <v>2369</v>
       </c>
@@ -91222,7 +91223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2442" spans="1:10">
+    <row r="2442" spans="1:10" hidden="1">
       <c r="A2442" t="s">
         <v>2371</v>
       </c>
@@ -91439,7 +91440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2449" spans="1:10">
+    <row r="2449" spans="1:10" hidden="1">
       <c r="A2449" t="s">
         <v>4208</v>
       </c>
@@ -91622,7 +91623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2455" spans="1:10">
+    <row r="2455" spans="1:10" hidden="1">
       <c r="A2455" t="s">
         <v>4342</v>
       </c>
@@ -91870,7 +91871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2463" spans="1:10">
+    <row r="2463" spans="1:10" hidden="1">
       <c r="A2463" t="s">
         <v>2415</v>
       </c>
@@ -92428,7 +92429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2481" spans="1:10">
+    <row r="2481" spans="1:10" hidden="1">
       <c r="A2481" t="s">
         <v>1952</v>
       </c>
@@ -93947,7 +93948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2530" spans="1:10">
+    <row r="2530" spans="1:10" hidden="1">
       <c r="A2530" t="s">
         <v>4349</v>
       </c>
@@ -93975,7 +93976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2531" spans="1:10">
+    <row r="2531" spans="1:10" hidden="1">
       <c r="A2531" t="s">
         <v>4191</v>
       </c>
@@ -94127,7 +94128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2536" spans="1:10">
+    <row r="2536" spans="1:10" hidden="1">
       <c r="A2536" t="s">
         <v>1406</v>
       </c>
@@ -94158,7 +94159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2537" spans="1:10">
+    <row r="2537" spans="1:10" hidden="1">
       <c r="A2537" t="s">
         <v>1408</v>
       </c>
@@ -94313,7 +94314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2542" spans="1:10">
+    <row r="2542" spans="1:10" hidden="1">
       <c r="A2542" t="s">
         <v>1404</v>
       </c>
@@ -94344,7 +94345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2543" spans="1:10">
+    <row r="2543" spans="1:10" hidden="1">
       <c r="A2543" t="s">
         <v>1410</v>
       </c>
@@ -94375,7 +94376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2544" spans="1:10">
+    <row r="2544" spans="1:10" hidden="1">
       <c r="A2544" t="s">
         <v>1412</v>
       </c>
@@ -94406,7 +94407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2545" spans="1:10">
+    <row r="2545" spans="1:10" hidden="1">
       <c r="A2545" t="s">
         <v>1416</v>
       </c>
@@ -94437,7 +94438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2546" spans="1:10">
+    <row r="2546" spans="1:10" hidden="1">
       <c r="A2546" t="s">
         <v>1414</v>
       </c>
@@ -94685,7 +94686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2554" spans="1:10">
+    <row r="2554" spans="1:10" hidden="1">
       <c r="A2554" t="s">
         <v>2619</v>
       </c>
@@ -94747,7 +94748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2556" spans="1:10">
+    <row r="2556" spans="1:10" hidden="1">
       <c r="A2556" t="s">
         <v>2921</v>
       </c>
@@ -94778,7 +94779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2557" spans="1:10">
+    <row r="2557" spans="1:10" hidden="1">
       <c r="A2557" t="s">
         <v>4066</v>
       </c>
@@ -95057,7 +95058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2566" spans="1:10">
+    <row r="2566" spans="1:10" hidden="1">
       <c r="A2566" t="s">
         <v>4589</v>
       </c>
@@ -95088,7 +95089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2567" spans="1:10">
+    <row r="2567" spans="1:10" hidden="1">
       <c r="A2567" t="s">
         <v>4590</v>
       </c>
@@ -95119,7 +95120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2568" spans="1:10">
+    <row r="2568" spans="1:10" hidden="1">
       <c r="A2568" t="s">
         <v>4591</v>
       </c>
@@ -95150,7 +95151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2569" spans="1:10">
+    <row r="2569" spans="1:10" hidden="1">
       <c r="A2569" t="s">
         <v>4592</v>
       </c>
@@ -95181,7 +95182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2570" spans="1:10">
+    <row r="2570" spans="1:10" hidden="1">
       <c r="A2570" t="s">
         <v>4593</v>
       </c>
@@ -95212,7 +95213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2571" spans="1:10">
+    <row r="2571" spans="1:10" hidden="1">
       <c r="A2571" t="s">
         <v>4088</v>
       </c>
@@ -95243,7 +95244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2572" spans="1:10">
+    <row r="2572" spans="1:10" hidden="1">
       <c r="A2572" t="s">
         <v>4594</v>
       </c>
@@ -95274,7 +95275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2573" spans="1:10">
+    <row r="2573" spans="1:10" hidden="1">
       <c r="A2573" t="s">
         <v>4595</v>
       </c>
@@ -95336,7 +95337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2575" spans="1:10">
+    <row r="2575" spans="1:10" hidden="1">
       <c r="A2575" t="s">
         <v>4596</v>
       </c>
@@ -95367,7 +95368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2576" spans="1:10">
+    <row r="2576" spans="1:10" hidden="1">
       <c r="A2576" t="s">
         <v>4597</v>
       </c>
@@ -95398,7 +95399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2577" spans="1:10">
+    <row r="2577" spans="1:10" hidden="1">
       <c r="A2577" t="s">
         <v>4598</v>
       </c>
@@ -95429,7 +95430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2578" spans="1:10">
+    <row r="2578" spans="1:10" hidden="1">
       <c r="A2578" t="s">
         <v>3976</v>
       </c>
@@ -95553,7 +95554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2582" spans="1:10">
+    <row r="2582" spans="1:10" hidden="1">
       <c r="A2582" t="s">
         <v>4587</v>
       </c>
@@ -95677,7 +95678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2586" spans="1:10">
+    <row r="2586" spans="1:10" hidden="1">
       <c r="A2586" t="s">
         <v>4102</v>
       </c>
@@ -96979,7 +96980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2628" spans="1:10">
+    <row r="2628" spans="1:10" hidden="1">
       <c r="A2628" t="s">
         <v>4192</v>
       </c>
@@ -97193,7 +97194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2635" spans="1:10">
+    <row r="2635" spans="1:10" hidden="1">
       <c r="A2635" t="s">
         <v>4193</v>
       </c>
@@ -97593,7 +97594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2648" spans="1:10">
+    <row r="2648" spans="1:10" hidden="1">
       <c r="A2648" t="s">
         <v>1810</v>
       </c>
@@ -97686,7 +97687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2651" spans="1:10">
+    <row r="2651" spans="1:10" hidden="1">
       <c r="A2651" t="s">
         <v>4194</v>
       </c>
@@ -97931,7 +97932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2659" spans="1:10">
+    <row r="2659" spans="1:10" hidden="1">
       <c r="A2659" t="s">
         <v>1455</v>
       </c>
@@ -97963,7 +97964,830 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:J2659"/>
+  <autoFilter ref="A7:J2659">
+    <filterColumn colId="6">
+      <filters>
+        <filter val="$ 1.001.000,00"/>
+        <filter val="$ 1.003.800,00"/>
+        <filter val="$ 1.004.640,00"/>
+        <filter val="$ 1.008.000,00"/>
+        <filter val="$ 1.017.002,00"/>
+        <filter val="$ 1.019.200,00"/>
+        <filter val="$ 1.022.000,00"/>
+        <filter val="$ 1.036.000,00"/>
+        <filter val="$ 1.043.000,00"/>
+        <filter val="$ 1.050.000,00"/>
+        <filter val="$ 1.054.200,00"/>
+        <filter val="$ 1.059.968,00"/>
+        <filter val="$ 1.064.000,00"/>
+        <filter val="$ 1.071.000,00"/>
+        <filter val="$ 1.077.440,00"/>
+        <filter val="$ 1.078.000,00"/>
+        <filter val="$ 1.085.000,00"/>
+        <filter val="$ 1.085.014,00"/>
+        <filter val="$ 1.089.088,00"/>
+        <filter val="$ 1.092.000,00"/>
+        <filter val="$ 1.095.766,00"/>
+        <filter val="$ 1.098.342,00"/>
+        <filter val="$ 1.106.000,00"/>
+        <filter val="$ 1.113.000,00"/>
+        <filter val="$ 1.120.000,00"/>
+        <filter val="$ 1.132.180,00"/>
+        <filter val="$ 1.134.000,00"/>
+        <filter val="$ 1.147.916,00"/>
+        <filter val="$ 1.148.000,00"/>
+        <filter val="$ 1.150.240,00"/>
+        <filter val="$ 1.155.000,00"/>
+        <filter val="$ 1.162.000,00"/>
+        <filter val="$ 1.164.800,00"/>
+        <filter val="$ 1.171.870,00"/>
+        <filter val="$ 1.173.466,00"/>
+        <filter val="$ 1.176.000,00"/>
+        <filter val="$ 1.179.360,00"/>
+        <filter val="$ 1.180.200,00"/>
+        <filter val="$ 1.185.184,00"/>
+        <filter val="$ 1.190.000,00"/>
+        <filter val="$ 1.193.514,00"/>
+        <filter val="$ 1.204.000,00"/>
+        <filter val="$ 1.208.480,00"/>
+        <filter val="$ 1.218.000,00"/>
+        <filter val="$ 1.223.040,00"/>
+        <filter val="$ 1.226.540,00"/>
+        <filter val="$ 1.232.000,00"/>
+        <filter val="$ 1.237.600,00"/>
+        <filter val="$ 1.241.800,00"/>
+        <filter val="$ 1.242.262,00"/>
+        <filter val="$ 1.246.000,00"/>
+        <filter val="$ 1.260.000,00"/>
+        <filter val="$ 1.265.628,00"/>
+        <filter val="$ 1.278.396,00"/>
+        <filter val="$ 1.279.992,00"/>
+        <filter val="$ 1.281.280,00"/>
+        <filter val="$ 1.302.000,00"/>
+        <filter val="$ 1.314.922,00"/>
+        <filter val="$ 1.316.000,00"/>
+        <filter val="$ 1.323.000,00"/>
+        <filter val="$ 1.330.000,00"/>
+        <filter val="$ 1.336.608,00"/>
+        <filter val="$ 1.344.000,00"/>
+        <filter val="$ 1.351.000,00"/>
+        <filter val="$ 1.354.080,00"/>
+        <filter val="$ 1.354.486,00"/>
+        <filter val="$ 1.358.000,00"/>
+        <filter val="$ 1.366.484,00"/>
+        <filter val="$ 1.369.704,00"/>
+        <filter val="$ 1.372.000,00"/>
+        <filter val="$ 1.380.666,00"/>
+        <filter val="$ 1.383.200,00"/>
+        <filter val="$ 1.386.000,00"/>
+        <filter val="$ 1.393.000,00"/>
+        <filter val="$ 1.400.000,00"/>
+        <filter val="$ 1.404.200,00"/>
+        <filter val="$ 1.416.800,00"/>
+        <filter val="$ 1.421.000,00"/>
+        <filter val="$ 1.425.424,00"/>
+        <filter val="$ 1.428.000,00"/>
+        <filter val="$ 1.441.440,00"/>
+        <filter val="$ 1.458.800,00"/>
+        <filter val="$ 1.470.000,00"/>
+        <filter val="$ 1.473.472,00"/>
+        <filter val="$ 1.484.000,00"/>
+        <filter val="$ 1.499.680,00"/>
+        <filter val="$ 1.512.000,00"/>
+        <filter val="$ 1.520.400,00"/>
+        <filter val="$ 1.521.520,00"/>
+        <filter val="$ 1.526.000,00"/>
+        <filter val="$ 1.540.000,00"/>
+        <filter val="$ 1.556.758,00"/>
+        <filter val="$ 1.557.920,00"/>
+        <filter val="$ 1.561.490,00"/>
+        <filter val="$ 1.568.000,00"/>
+        <filter val="$ 1.569.568,00"/>
+        <filter val="$ 1.572.480,00"/>
+        <filter val="$ 1.582.000,00"/>
+        <filter val="$ 1.587.040,00"/>
+        <filter val="$ 1.589.000,00"/>
+        <filter val="$ 1.596.000,00"/>
+        <filter val="$ 1.597.400,00"/>
+        <filter val="$ 1.601.600,00"/>
+        <filter val="$ 1.608.642,00"/>
+        <filter val="$ 1.610.000,00"/>
+        <filter val="$ 1.624.000,00"/>
+        <filter val="$ 1.625.946,00"/>
+        <filter val="$ 1.633.632,00"/>
+        <filter val="$ 1.638.000,00"/>
+        <filter val="$ 1.643.236,00"/>
+        <filter val="$ 1.645.280,00"/>
+        <filter val="$ 1.651.104,00"/>
+        <filter val="$ 1.660.540,00"/>
+        <filter val="$ 1.666.000,00"/>
+        <filter val="$ 1.671.600,00"/>
+        <filter val="$ 1.674.400,00"/>
+        <filter val="$ 1.680.000,00"/>
+        <filter val="$ 1.718.080,00"/>
+        <filter val="$ 1.732.640,00"/>
+        <filter val="$ 1.747.200,00"/>
+        <filter val="$ 1.750.000,00"/>
+        <filter val="$ 1.778.000,00"/>
+        <filter val="$ 1.793.792,00"/>
+        <filter val="$ 1.808.016,00"/>
+        <filter val="$ 1.820.000,00"/>
+        <filter val="$ 1.841.840,00"/>
+        <filter val="$ 1.855.000,00"/>
+        <filter val="$ 1.876.000,00"/>
+        <filter val="$ 1.890.000,00"/>
+        <filter val="$ 1.892.800,00"/>
+        <filter val="$ 1.901.200,00"/>
+        <filter val="$ 1.904.000,00"/>
+        <filter val="$ 1.918.000,00"/>
+        <filter val="$ 1.918.420,00"/>
+        <filter val="$ 1.921.920,00"/>
+        <filter val="$ 1.946.000,00"/>
+        <filter val="$ 1.950.200,00"/>
+        <filter val="$ 1.953.000,00"/>
+        <filter val="$ 1.960.000,00"/>
+        <filter val="$ 1.965.600,00"/>
+        <filter val="$ 1.988.000,00"/>
+        <filter val="$ 10.192,00"/>
+        <filter val="$ 10.192.000,00"/>
+        <filter val="$ 10.220,00"/>
+        <filter val="$ 10.430.000,00"/>
+        <filter val="$ 10.500,00"/>
+        <filter val="$ 10.920,00"/>
+        <filter val="$ 100.800,00"/>
+        <filter val="$ 101.920,00"/>
+        <filter val="$ 102.200,00"/>
+        <filter val="$ 102.214,00"/>
+        <filter val="$ 103.782,00"/>
+        <filter val="$ 104.104,00"/>
+        <filter val="$ 108.906,00"/>
+        <filter val="$ 109.200,00"/>
+        <filter val="$ 109.522,00"/>
+        <filter val="$ 11.060.000,00"/>
+        <filter val="$ 11.065.600,00"/>
+        <filter val="$ 11.200,00"/>
+        <filter val="$ 11.211.200,00"/>
+        <filter val="$ 11.648,00"/>
+        <filter val="$ 11.648.000,00"/>
+        <filter val="$ 11.732,00"/>
+        <filter val="$ 11.760.000,00"/>
+        <filter val="$ 11.830.000,00"/>
+        <filter val="$ 11.900.000,00"/>
+        <filter val="$ 110.600,00"/>
+        <filter val="$ 112.000,00"/>
+        <filter val="$ 112.112,00"/>
+        <filter val="$ 112.434,00"/>
+        <filter val="$ 114.170,00"/>
+        <filter val="$ 114.800,00"/>
+        <filter val="$ 116.200,00"/>
+        <filter val="$ 117.600,00"/>
+        <filter val="$ 119.000,00"/>
+        <filter val="$ 12.230.400,00"/>
+        <filter val="$ 12.376,00"/>
+        <filter val="$ 12.460.000,00"/>
+        <filter val="$ 12.586,00"/>
+        <filter val="$ 12.600,00"/>
+        <filter val="$ 12.880.000,00"/>
+        <filter val="$ 120.120,00"/>
+        <filter val="$ 120.400,00"/>
+        <filter val="$ 121.086,00"/>
+        <filter val="$ 121.716,00"/>
+        <filter val="$ 121.800,00"/>
+        <filter val="$ 122.304,00"/>
+        <filter val="$ 125.174,00"/>
+        <filter val="$ 125.804,00"/>
+        <filter val="$ 126.000,00"/>
+        <filter val="$ 127.400,00"/>
+        <filter val="$ 128.128,00"/>
+        <filter val="$ 128.800,00"/>
+        <filter val="$ 13.104,00"/>
+        <filter val="$ 13.160.000,00"/>
+        <filter val="$ 13.832,00"/>
+        <filter val="$ 13.860.000,00"/>
+        <filter val="$ 130.200,00"/>
+        <filter val="$ 131.040,00"/>
+        <filter val="$ 131.040.000,00"/>
+        <filter val="$ 131.334,00"/>
+        <filter val="$ 131.460,00"/>
+        <filter val="$ 133.000,00"/>
+        <filter val="$ 136.136,00"/>
+        <filter val="$ 137.200,00"/>
+        <filter val="$ 138.376,00"/>
+        <filter val="$ 138.600,00"/>
+        <filter val="$ 14.000,00"/>
+        <filter val="$ 14.000.000,00"/>
+        <filter val="$ 14.420.000,00"/>
+        <filter val="$ 14.560.000,00"/>
+        <filter val="$ 14.700.000,00"/>
+        <filter val="$ 140.000,00"/>
+        <filter val="$ 140.112,00"/>
+        <filter val="$ 141.526,00"/>
+        <filter val="$ 142.548,00"/>
+        <filter val="$ 142.688,00"/>
+        <filter val="$ 144.144,00"/>
+        <filter val="$ 145.600,00"/>
+        <filter val="$ 148.400,00"/>
+        <filter val="$ 149.380,00"/>
+        <filter val="$ 15.260.000,00"/>
+        <filter val="$ 15.400,00"/>
+        <filter val="$ 15.568,00"/>
+        <filter val="$ 15.652,00"/>
+        <filter val="$ 15.680.000,00"/>
+        <filter val="$ 15.960.000,00"/>
+        <filter val="$ 154.000,00"/>
+        <filter val="$ 155.680,00"/>
+        <filter val="$ 156.464,00"/>
+        <filter val="$ 157.248,00"/>
+        <filter val="$ 16.100.000,00"/>
+        <filter val="$ 16.310.000,00"/>
+        <filter val="$ 16.800,00"/>
+        <filter val="$ 16.800.000,00"/>
+        <filter val="$ 160.160,00"/>
+        <filter val="$ 161.000,00"/>
+        <filter val="$ 164.318,00"/>
+        <filter val="$ 167.440,00"/>
+        <filter val="$ 168.000,00"/>
+        <filter val="$ 17.304,00"/>
+        <filter val="$ 17.472,00"/>
+        <filter val="$ 17.920,00"/>
+        <filter val="$ 171.234,00"/>
+        <filter val="$ 172.200,00"/>
+        <filter val="$ 172.970,00"/>
+        <filter val="$ 174.720,00"/>
+        <filter val="$ 175.000,00"/>
+        <filter val="$ 176.176,00"/>
+        <filter val="$ 179.200,00"/>
+        <filter val="$ 18.200,00"/>
+        <filter val="$ 18.788,00"/>
+        <filter val="$ 18.802,00"/>
+        <filter val="$ 18.872,00"/>
+        <filter val="$ 18.928,00"/>
+        <filter val="$ 180.600,00"/>
+        <filter val="$ 182.000,00"/>
+        <filter val="$ 186.802,00"/>
+        <filter val="$ 188.692,00"/>
+        <filter val="$ 189.000,00"/>
+        <filter val="$ 189.280,00"/>
+        <filter val="$ 19.026,00"/>
+        <filter val="$ 19.460.000,00"/>
+        <filter val="$ 19.600.000,00"/>
+        <filter val="$ 190.274,00"/>
+        <filter val="$ 194.600,00"/>
+        <filter val="$ 196.000,00"/>
+        <filter val="$ 196.560,00"/>
+        <filter val="$ 2.002.000,00"/>
+        <filter val="$ 2.016.000,00"/>
+        <filter val="$ 2.028.502,00"/>
+        <filter val="$ 2.030.000,00"/>
+        <filter val="$ 2.038.400,00"/>
+        <filter val="$ 2.039.800,00"/>
+        <filter val="$ 2.044.000,00"/>
+        <filter val="$ 2.046.800,00"/>
+        <filter val="$ 2.054.570,00"/>
+        <filter val="$ 2.065.000,00"/>
+        <filter val="$ 2.079.000,00"/>
+        <filter val="$ 2.086.000,00"/>
+        <filter val="$ 2.091.404,00"/>
+        <filter val="$ 2.100.000,00"/>
+        <filter val="$ 2.102.800,00"/>
+        <filter val="$ 2.111.200,00"/>
+        <filter val="$ 2.128.000,00"/>
+        <filter val="$ 2.130.660,00"/>
+        <filter val="$ 2.136.750,00"/>
+        <filter val="$ 2.140.320,00"/>
+        <filter val="$ 2.156.000,00"/>
+        <filter val="$ 2.163.000,00"/>
+        <filter val="$ 2.169.440,00"/>
+        <filter val="$ 2.170.000,00"/>
+        <filter val="$ 2.177.000,00"/>
+        <filter val="$ 2.184.000,00"/>
+        <filter val="$ 2.198.000,00"/>
+        <filter val="$ 2.205.000,00"/>
+        <filter val="$ 2.226.000,00"/>
+        <filter val="$ 2.240.000,00"/>
+        <filter val="$ 2.256.800,00"/>
+        <filter val="$ 2.268.238,00"/>
+        <filter val="$ 2.275.000,00"/>
+        <filter val="$ 2.282.000,00"/>
+        <filter val="$ 2.295.818,00"/>
+        <filter val="$ 2.296.112,00"/>
+        <filter val="$ 2.300.480,00"/>
+        <filter val="$ 2.310.000,00"/>
+        <filter val="$ 2.315.040,00"/>
+        <filter val="$ 2.317.000,00"/>
+        <filter val="$ 2.329.600,00"/>
+        <filter val="$ 2.338.000,00"/>
+        <filter val="$ 2.366.000,00"/>
+        <filter val="$ 2.380.000,00"/>
+        <filter val="$ 2.383.318,00"/>
+        <filter val="$ 2.402.400,00"/>
+        <filter val="$ 2.435.062,00"/>
+        <filter val="$ 2.436.000,00"/>
+        <filter val="$ 2.449.076,00"/>
+        <filter val="$ 2.460.640,00"/>
+        <filter val="$ 2.464.000,00"/>
+        <filter val="$ 2.468.788,00"/>
+        <filter val="$ 2.475.200,00"/>
+        <filter val="$ 2.478.000,00"/>
+        <filter val="$ 2.504.320,00"/>
+        <filter val="$ 2.506.000,00"/>
+        <filter val="$ 2.520.000,00"/>
+        <filter val="$ 2.569.000,00"/>
+        <filter val="$ 2.590.000,00"/>
+        <filter val="$ 2.591.680,00"/>
+        <filter val="$ 2.594.592,00"/>
+        <filter val="$ 2.604.000,00"/>
+        <filter val="$ 2.606.240,00"/>
+        <filter val="$ 2.629.858,00"/>
+        <filter val="$ 2.632.000,00"/>
+        <filter val="$ 2.633.904,00"/>
+        <filter val="$ 2.646.000,00"/>
+        <filter val="$ 2.660.000,00"/>
+        <filter val="$ 2.674.000,00"/>
+        <filter val="$ 2.693.600,00"/>
+        <filter val="$ 2.716.000,00"/>
+        <filter val="$ 2.730.000,00"/>
+        <filter val="$ 2.739.450,00"/>
+        <filter val="$ 2.751.840,00"/>
+        <filter val="$ 2.777.796,00"/>
+        <filter val="$ 2.779.000,00"/>
+        <filter val="$ 2.786.000,00"/>
+        <filter val="$ 2.799.020,00"/>
+        <filter val="$ 2.800.000,00"/>
+        <filter val="$ 2.870.000,00"/>
+        <filter val="$ 2.897.440,00"/>
+        <filter val="$ 2.933.000,00"/>
+        <filter val="$ 2.940.000,00"/>
+        <filter val="$ 2.942.156,00"/>
+        <filter val="$ 2.954.000,00"/>
+        <filter val="$ 2.958.606,00"/>
+        <filter val="$ 2.984.800,00"/>
+        <filter val="$ 20.238.400,00"/>
+        <filter val="$ 20.328,00"/>
+        <filter val="$ 20.384,00"/>
+        <filter val="$ 203.000,00"/>
+        <filter val="$ 203.406,00"/>
+        <filter val="$ 203.840,00"/>
+        <filter val="$ 204.400,00"/>
+        <filter val="$ 204.428,00"/>
+        <filter val="$ 208.208,00"/>
+        <filter val="$ 21.000,00"/>
+        <filter val="$ 210.000,00"/>
+        <filter val="$ 218.400,00"/>
+        <filter val="$ 22.400,00"/>
+        <filter val="$ 22.484,00"/>
+        <filter val="$ 220.150,00"/>
+        <filter val="$ 224.000,00"/>
+        <filter val="$ 224.224,00"/>
+        <filter val="$ 224.868,00"/>
+        <filter val="$ 23.150.400,00"/>
+        <filter val="$ 23.296,00"/>
+        <filter val="$ 23.464,00"/>
+        <filter val="$ 23.590,00"/>
+        <filter val="$ 23.660.000,00"/>
+        <filter val="$ 23.800,00"/>
+        <filter val="$ 230.048,00"/>
+        <filter val="$ 231.000,00"/>
+        <filter val="$ 232.232,00"/>
+        <filter val="$ 233.520,00"/>
+        <filter val="$ 233.800,00"/>
+        <filter val="$ 234.696,00"/>
+        <filter val="$ 235.872,00"/>
+        <filter val="$ 236.600,00"/>
+        <filter val="$ 238.000,00"/>
+        <filter val="$ 24.220,00"/>
+        <filter val="$ 240.590,00"/>
+        <filter val="$ 247.520,00"/>
+        <filter val="$ 25.158,00"/>
+        <filter val="$ 25.200,00"/>
+        <filter val="$ 25.200.000,00"/>
+        <filter val="$ 25.900.000,00"/>
+        <filter val="$ 25.942,00"/>
+        <filter val="$ 250.026,00"/>
+        <filter val="$ 251.594,00"/>
+        <filter val="$ 252.000,00"/>
+        <filter val="$ 258.160,00"/>
+        <filter val="$ 259.462,00"/>
+        <filter val="$ 26.208,00"/>
+        <filter val="$ 26.208.000,00"/>
+        <filter val="$ 26.600,00"/>
+        <filter val="$ 26.726,00"/>
+        <filter val="$ 260.400,00"/>
+        <filter val="$ 266.000,00"/>
+        <filter val="$ 269.360,00"/>
+        <filter val="$ 27.664,00"/>
+        <filter val="$ 27.678,00"/>
+        <filter val="$ 27.860.000,00"/>
+        <filter val="$ 273.000,00"/>
+        <filter val="$ 275.184,00"/>
+        <filter val="$ 276.640,00"/>
+        <filter val="$ 28.000,00"/>
+        <filter val="$ 28.000.000,00"/>
+        <filter val="$ 280.000,00"/>
+        <filter val="$ 281.470,00"/>
+        <filter val="$ 281.638,00"/>
+        <filter val="$ 283.052,00"/>
+        <filter val="$ 283.920,00"/>
+        <filter val="$ 287.000,00"/>
+        <filter val="$ 288.288,00"/>
+        <filter val="$ 29.120,00"/>
+        <filter val="$ 29.400,00"/>
+        <filter val="$ 29.414,00"/>
+        <filter val="$ 291.200,00"/>
+        <filter val="$ 294.000,00"/>
+        <filter val="$ 296.800,00"/>
+        <filter val="$ 298.774,00"/>
+        <filter val="$ 3.010.000,00"/>
+        <filter val="$ 3.066.000,00"/>
+        <filter val="$ 3.080.000,00"/>
+        <filter val="$ 3.096.800,00"/>
+        <filter val="$ 3.136.000,00"/>
+        <filter val="$ 3.138.296,00"/>
+        <filter val="$ 3.150.000,00"/>
+        <filter val="$ 3.188.640,00"/>
+        <filter val="$ 3.203.200,00"/>
+        <filter val="$ 3.206.000,00"/>
+        <filter val="$ 3.220.000,00"/>
+        <filter val="$ 3.262.000,00"/>
+        <filter val="$ 3.276.000,00"/>
+        <filter val="$ 3.290.000,00"/>
+        <filter val="$ 3.334.240,00"/>
+        <filter val="$ 3.348.800,00"/>
+        <filter val="$ 3.360.000,00"/>
+        <filter val="$ 3.385.200,00"/>
+        <filter val="$ 3.402.000,00"/>
+        <filter val="$ 3.421.600,00"/>
+        <filter val="$ 3.430.000,00"/>
+        <filter val="$ 3.472.000,00"/>
+        <filter val="$ 3.486.000,00"/>
+        <filter val="$ 3.493.000,00"/>
+        <filter val="$ 3.494.400,00"/>
+        <filter val="$ 3.500.000,00"/>
+        <filter val="$ 3.554.600,00"/>
+        <filter val="$ 3.567.200,00"/>
+        <filter val="$ 3.570.000,00"/>
+        <filter val="$ 3.616.704,00"/>
+        <filter val="$ 3.626.000,00"/>
+        <filter val="$ 3.640.000,00"/>
+        <filter val="$ 3.654.000,00"/>
+        <filter val="$ 3.682.000,00"/>
+        <filter val="$ 3.710.000,00"/>
+        <filter val="$ 3.755.066,00"/>
+        <filter val="$ 3.773.952,00"/>
+        <filter val="$ 3.814.720,00"/>
+        <filter val="$ 3.822.000,00"/>
+        <filter val="$ 3.850.000,00"/>
+        <filter val="$ 3.864.000,00"/>
+        <filter val="$ 3.906.000,00"/>
+        <filter val="$ 3.920.000,00"/>
+        <filter val="$ 3.927.000,00"/>
+        <filter val="$ 3.948.000,00"/>
+        <filter val="$ 3.956.974,00"/>
+        <filter val="$ 3.990.000,00"/>
+        <filter val="$ 30.800,00"/>
+        <filter val="$ 301.000,00"/>
+        <filter val="$ 305.760,00"/>
+        <filter val="$ 306.628,00"/>
+        <filter val="$ 308.000,00"/>
+        <filter val="$ 31.290,00"/>
+        <filter val="$ 31.444,00"/>
+        <filter val="$ 314.496,00"/>
+        <filter val="$ 32.032,00"/>
+        <filter val="$ 32.200,00"/>
+        <filter val="$ 320.320,00"/>
+        <filter val="$ 322.000,00"/>
+        <filter val="$ 33.600,00"/>
+        <filter val="$ 330.218,00"/>
+        <filter val="$ 336.000,00"/>
+        <filter val="$ 337.946,00"/>
+        <filter val="$ 34.594,00"/>
+        <filter val="$ 34.944,00"/>
+        <filter val="$ 343.000,00"/>
+        <filter val="$ 344.218,00"/>
+        <filter val="$ 345.940,00"/>
+        <filter val="$ 35.000,00"/>
+        <filter val="$ 350.000,00"/>
+        <filter val="$ 352.352,00"/>
+        <filter val="$ 353.808,00"/>
+        <filter val="$ 357.000,00"/>
+        <filter val="$ 36.400,00"/>
+        <filter val="$ 361.508,00"/>
+        <filter val="$ 361.676,00"/>
+        <filter val="$ 364.000,00"/>
+        <filter val="$ 37.744,00"/>
+        <filter val="$ 37.856,00"/>
+        <filter val="$ 37.856.000,00"/>
+        <filter val="$ 371.000,00"/>
+        <filter val="$ 377.398,00"/>
+        <filter val="$ 378.000,00"/>
+        <filter val="$ 378.560,00"/>
+        <filter val="$ 38.066,00"/>
+        <filter val="$ 385.000,00"/>
+        <filter val="$ 385.252,00"/>
+        <filter val="$ 39.200,00"/>
+        <filter val="$ 39.312,00"/>
+        <filter val="$ 392.000,00"/>
+        <filter val="$ 393.120,00"/>
+        <filter val="$ 4.004.000,00"/>
+        <filter val="$ 4.006.912,00"/>
+        <filter val="$ 4.158.000,00"/>
+        <filter val="$ 4.200.000,00"/>
+        <filter val="$ 4.207.840,00"/>
+        <filter val="$ 4.222.400,00"/>
+        <filter val="$ 4.295.200,00"/>
+        <filter val="$ 4.340.000,00"/>
+        <filter val="$ 4.368,00"/>
+        <filter val="$ 4.414.200,00"/>
+        <filter val="$ 4.480.000,00"/>
+        <filter val="$ 4.513.600,00"/>
+        <filter val="$ 4.659.200,00"/>
+        <filter val="$ 4.732.000,00"/>
+        <filter val="$ 4.746.560,00"/>
+        <filter val="$ 4.760.000,00"/>
+        <filter val="$ 4.900.000,00"/>
+        <filter val="$ 4.950.400,00"/>
+        <filter val="$ 40.600,00"/>
+        <filter val="$ 40.768,00"/>
+        <filter val="$ 406.000,00"/>
+        <filter val="$ 406.812,00"/>
+        <filter val="$ 41.510,00"/>
+        <filter val="$ 41.636,00"/>
+        <filter val="$ 413.000,00"/>
+        <filter val="$ 415.128,00"/>
+        <filter val="$ 42.000,00"/>
+        <filter val="$ 420.000,00"/>
+        <filter val="$ 422.240,00"/>
+        <filter val="$ 422.450,00"/>
+        <filter val="$ 427.000,00"/>
+        <filter val="$ 43.246,00"/>
+        <filter val="$ 43.400,00"/>
+        <filter val="$ 434.000,00"/>
+        <filter val="$ 436.800,00"/>
+        <filter val="$ 44.800,00"/>
+        <filter val="$ 44.982,00"/>
+        <filter val="$ 444.080,00"/>
+        <filter val="$ 448.000,00"/>
+        <filter val="$ 448.154,00"/>
+        <filter val="$ 45.402,00"/>
+        <filter val="$ 451.360,00"/>
+        <filter val="$ 453.740,00"/>
+        <filter val="$ 456.022,00"/>
+        <filter val="$ 46.200,00"/>
+        <filter val="$ 461.566,00"/>
+        <filter val="$ 462.000,00"/>
+        <filter val="$ 465.920,00"/>
+        <filter val="$ 469.000,00"/>
+        <filter val="$ 47.180,00"/>
+        <filter val="$ 47.600,00"/>
+        <filter val="$ 471.744,00"/>
+        <filter val="$ 476.000,00"/>
+        <filter val="$ 48.048,00"/>
+        <filter val="$ 480.480,00"/>
+        <filter val="$ 483.000,00"/>
+        <filter val="$ 49.000,00"/>
+        <filter val="$ 490.000,00"/>
+        <filter val="$ 5.023.200,00"/>
+        <filter val="$ 5.040.000,00"/>
+        <filter val="$ 5.096.000,00"/>
+        <filter val="$ 5.166.000,00"/>
+        <filter val="$ 5.180.000,00"/>
+        <filter val="$ 5.241.600,00"/>
+        <filter val="$ 5.306.000,00"/>
+        <filter val="$ 5.372.640,00"/>
+        <filter val="$ 5.460.000,00"/>
+        <filter val="$ 5.561.920,00"/>
+        <filter val="$ 5.586.000,00"/>
+        <filter val="$ 5.600,00"/>
+        <filter val="$ 5.600.000,00"/>
+        <filter val="$ 5.670.000,00"/>
+        <filter val="$ 5.678.400,00"/>
+        <filter val="$ 5.752.824,00"/>
+        <filter val="$ 5.824,00"/>
+        <filter val="$ 5.824.000,00"/>
+        <filter val="$ 5.880.000,00"/>
+        <filter val="$ 50.400,00"/>
+        <filter val="$ 501.620,00"/>
+        <filter val="$ 503.188,00"/>
+        <filter val="$ 504.000,00"/>
+        <filter val="$ 51.800,00"/>
+        <filter val="$ 51.898,00"/>
+        <filter val="$ 511.000,00"/>
+        <filter val="$ 518.000,00"/>
+        <filter val="$ 523.600,00"/>
+        <filter val="$ 524.160,00"/>
+        <filter val="$ 53.200,00"/>
+        <filter val="$ 532.000,00"/>
+        <filter val="$ 534.800,00"/>
+        <filter val="$ 546.000,00"/>
+        <filter val="$ 547.610,00"/>
+        <filter val="$ 55.328,00"/>
+        <filter val="$ 55.356,00"/>
+        <filter val="$ 553.000,00"/>
+        <filter val="$ 56.000,00"/>
+        <filter val="$ 56.784.000,00"/>
+        <filter val="$ 560.000,00"/>
+        <filter val="$ 563.262,00"/>
+        <filter val="$ 567.000,00"/>
+        <filter val="$ 574.000,00"/>
+        <filter val="$ 575.778,00"/>
+        <filter val="$ 58.240,00"/>
+        <filter val="$ 58.800,00"/>
+        <filter val="$ 581.000,00"/>
+        <filter val="$ 582.400,00"/>
+        <filter val="$ 588.000,00"/>
+        <filter val="$ 59.752,00"/>
+        <filter val="$ 597.548,00"/>
+        <filter val="$ 6.020.000,00"/>
+        <filter val="$ 6.115.200,00"/>
+        <filter val="$ 6.132.672,00"/>
+        <filter val="$ 6.160.000,00"/>
+        <filter val="$ 6.216.000,00"/>
+        <filter val="$ 6.440.000,00"/>
+        <filter val="$ 6.450.080,00"/>
+        <filter val="$ 6.552.000,00"/>
+        <filter val="$ 6.580.000,00"/>
+        <filter val="$ 6.720.000,00"/>
+        <filter val="$ 6.726.720,00"/>
+        <filter val="$ 6.828.640,00"/>
+        <filter val="$ 6.860.000,00"/>
+        <filter val="$ 6.916.000,00"/>
+        <filter val="$ 6.986.000,00"/>
+        <filter val="$ 60.424.000,00"/>
+        <filter val="$ 60.536,00"/>
+        <filter val="$ 602.000,00"/>
+        <filter val="$ 61.152,00"/>
+        <filter val="$ 61.600,00"/>
+        <filter val="$ 613.270,00"/>
+        <filter val="$ 616.000,00"/>
+        <filter val="$ 618.030,00"/>
+        <filter val="$ 621.124,00"/>
+        <filter val="$ 625.842,00"/>
+        <filter val="$ 628.992,00"/>
+        <filter val="$ 63.000,00"/>
+        <filter val="$ 630.000,00"/>
+        <filter val="$ 633.080,00"/>
+        <filter val="$ 637.000,00"/>
+        <filter val="$ 64.400,00"/>
+        <filter val="$ 640.640,00"/>
+        <filter val="$ 641.480,00"/>
+        <filter val="$ 644.000,00"/>
+        <filter val="$ 644.714,00"/>
+        <filter val="$ 65.520,00"/>
+        <filter val="$ 65.800,00"/>
+        <filter val="$ 658.000,00"/>
+        <filter val="$ 658.868,00"/>
+        <filter val="$ 669.760,00"/>
+        <filter val="$ 672.000,00"/>
+        <filter val="$ 68.600,00"/>
+        <filter val="$ 68.866,00"/>
+        <filter val="$ 680.400,00"/>
+        <filter val="$ 684.026,00"/>
+        <filter val="$ 686.000,00"/>
+        <filter val="$ 691.894,00"/>
+        <filter val="$ 693.000,00"/>
+        <filter val="$ 698.880,00"/>
+        <filter val="$ 7.000,00"/>
+        <filter val="$ 7.000.000,00"/>
+        <filter val="$ 7.098.000,00"/>
+        <filter val="$ 7.140.000,00"/>
+        <filter val="$ 7.280,00"/>
+        <filter val="$ 7.280.000,00"/>
+        <filter val="$ 7.411.040,00"/>
+        <filter val="$ 7.560.000,00"/>
+        <filter val="$ 7.571.200,00"/>
+        <filter val="$ 7.630.000,00"/>
+        <filter val="$ 7.700.000,00"/>
+        <filter val="$ 7.736.596,00"/>
+        <filter val="$ 7.868,00"/>
+        <filter val="$ 7.980.000,00"/>
+        <filter val="$ 70.000,00"/>
+        <filter val="$ 70.476,00"/>
+        <filter val="$ 700.000,00"/>
+        <filter val="$ 704.424,00"/>
+        <filter val="$ 704.704,00"/>
+        <filter val="$ 707.616,00"/>
+        <filter val="$ 71.400,00"/>
+        <filter val="$ 714.000,00"/>
+        <filter val="$ 716.800,00"/>
+        <filter val="$ 72.072,00"/>
+        <filter val="$ 72.660,00"/>
+        <filter val="$ 72.800,00"/>
+        <filter val="$ 721.000,00"/>
+        <filter val="$ 726.544,00"/>
+        <filter val="$ 728.000,00"/>
+        <filter val="$ 729.400,00"/>
+        <filter val="$ 735.000,00"/>
+        <filter val="$ 74.200,00"/>
+        <filter val="$ 742.000,00"/>
+        <filter val="$ 749.000,00"/>
+        <filter val="$ 752.752,00"/>
+        <filter val="$ 754.796,00"/>
+        <filter val="$ 756.000,00"/>
+        <filter val="$ 76.874,00"/>
+        <filter val="$ 760.970,00"/>
+        <filter val="$ 762.650,00"/>
+        <filter val="$ 763.000,00"/>
+        <filter val="$ 768.768,00"/>
+        <filter val="$ 77.000,00"/>
+        <filter val="$ 77.056,00"/>
+        <filter val="$ 77.840,00"/>
+        <filter val="$ 770.000,00"/>
+        <filter val="$ 770.518,00"/>
+        <filter val="$ 784.000,00"/>
+        <filter val="$ 786.800,00"/>
+        <filter val="$ 797.944,00"/>
+        <filter val="$ 798.000,00"/>
+        <filter val="$ 8.008.000,00"/>
+        <filter val="$ 8.092.000,00"/>
+        <filter val="$ 8.120.000,00"/>
+        <filter val="$ 8.226.400,00"/>
+        <filter val="$ 8.260.000,00"/>
+        <filter val="$ 8.400,00"/>
+        <filter val="$ 8.444.800,00"/>
+        <filter val="$ 8.565.648,00"/>
+        <filter val="$ 8.590.400,00"/>
+        <filter val="$ 8.736,00"/>
+        <filter val="$ 8.736.000,00"/>
+        <filter val="$ 8.960.000,00"/>
+        <filter val="$ 80.080,00"/>
+        <filter val="$ 800.800,00"/>
+        <filter val="$ 805.000,00"/>
+        <filter val="$ 812.000,00"/>
+        <filter val="$ 816.200,00"/>
+        <filter val="$ 825.552,00"/>
+        <filter val="$ 826.000,00"/>
+        <filter val="$ 830.270,00"/>
+        <filter val="$ 833.000,00"/>
+        <filter val="$ 84.000,00"/>
+        <filter val="$ 84.756,00"/>
+        <filter val="$ 840.000,00"/>
+        <filter val="$ 844.480,00"/>
+        <filter val="$ 845.292,00"/>
+        <filter val="$ 847.560,00"/>
+        <filter val="$ 849.142,00"/>
+        <filter val="$ 852.600,00"/>
+        <filter val="$ 854.000,00"/>
+        <filter val="$ 859.040,00"/>
+        <filter val="$ 86.492,00"/>
+        <filter val="$ 86.800,00"/>
+        <filter val="$ 860.538,00"/>
+        <filter val="$ 861.000,00"/>
+        <filter val="$ 864.864,00"/>
+        <filter val="$ 868.000,00"/>
+        <filter val="$ 87.360,00"/>
+        <filter val="$ 873.600,00"/>
+        <filter val="$ 88.200,00"/>
+        <filter val="$ 882.000,00"/>
+        <filter val="$ 882.168,00"/>
+        <filter val="$ 89.684,00"/>
+        <filter val="$ 896.000,00"/>
+        <filter val="$ 9.027.200,00"/>
+        <filter val="$ 9.172.800,00"/>
+        <filter val="$ 9.245.600,00"/>
+        <filter val="$ 9.318.400,00"/>
+        <filter val="$ 9.506.000,00"/>
+        <filter val="$ 9.520.000,00"/>
+        <filter val="$ 9.595.040,00"/>
+        <filter val="$ 9.646.000,00"/>
+        <filter val="$ 9.660.000,00"/>
+        <filter val="$ 9.786.000,00"/>
+        <filter val="$ 9.800,00"/>
+        <filter val="$ 9.800.000,00"/>
+        <filter val="$ 9.906.624,00"/>
+        <filter val="$ 904.400,00"/>
+        <filter val="$ 908.600,00"/>
+        <filter val="$ 91.000,00"/>
+        <filter val="$ 910.000,00"/>
+        <filter val="$ 911.260,00"/>
+        <filter val="$ 911.568,00"/>
+        <filter val="$ 912.044,00"/>
+        <filter val="$ 913.150,00"/>
+        <filter val="$ 915.824,00"/>
+        <filter val="$ 924.000,00"/>
+        <filter val="$ 927.766,00"/>
+        <filter val="$ 935.200,00"/>
+        <filter val="$ 938.000,00"/>
+        <filter val="$ 94.346,00"/>
+        <filter val="$ 94.640,00"/>
+        <filter val="$ 943.488,00"/>
+        <filter val="$ 944.944,00"/>
+        <filter val="$ 95.130,00"/>
+        <filter val="$ 95.200,00"/>
+        <filter val="$ 951.356,00"/>
+        <filter val="$ 952.000,00"/>
+        <filter val="$ 96.096,00"/>
+        <filter val="$ 96.600,00"/>
+        <filter val="$ 966.000,00"/>
+        <filter val="$ 967.400,00"/>
+        <filter val="$ 974.400,00"/>
+        <filter val="$ 974.932,00"/>
+        <filter val="$ 98.000,00"/>
+        <filter val="$ 98.602,00"/>
+        <filter val="$ 980.000,00"/>
+        <filter val="$ 999.614,00"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>